<commit_message>
Add contingencies, update animate
</commit_message>
<xml_diff>
--- a/static/example.xlsx
+++ b/static/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>id</t>
   </si>
@@ -28,6 +28,9 @@
     <t>request</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>Xuất Phát</t>
   </si>
   <si>
@@ -37,6 +40,9 @@
     <t>Quân Ai Cập đuổi tới rồi: mọi người chỉ kịp lấy hành lý quan trọng nhất mà chạy thôi! Mỗi người chơi hãy chọn 1 hành trang cho mình và giải thích chức năng hợp lý!</t>
   </si>
   <si>
+    <t>obstacle</t>
+  </si>
+  <si>
     <t>Hù ……. =))))))))</t>
   </si>
   <si>
@@ -47,6 +53,27 @@
   </si>
   <si>
     <t>Khát quá đi uống nước, uống xong đắng quá! Mỗi người 1 chén nước sau đó thể hiện cảm xúc uống phải NƯỚC ĐẮNG.</t>
+  </si>
+  <si>
+    <t>Toang rồi!</t>
+  </si>
+  <si>
+    <t>Bị Quận địch phục kích</t>
+  </si>
+  <si>
+    <t>Quay xí ngầu được mấy nút thì phải lui về mấy bước</t>
+  </si>
+  <si>
+    <t>contingency</t>
+  </si>
+  <si>
+    <t>Toang tập 2</t>
+  </si>
+  <si>
+    <t>Gặp thời tiết xấu</t>
+  </si>
+  <si>
+    <t>Các thành viên phải che đầu bằng tay hoặc bằng đồ vật trong 1 lượt tiếp theo kể từ bây giờ</t>
   </si>
 </sst>
 </file>
@@ -55,11 +82,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +95,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.8"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Fira Code"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -75,11 +108,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -91,69 +123,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,14 +154,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -190,8 +199,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,7 +231,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,19 +260,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,157 +434,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,15 +468,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,11 +504,29 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,129 +545,120 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -634,36 +667,39 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -985,20 +1021,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="8.6875" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
     <col min="3" max="3" width="22.53125" customWidth="1"/>
     <col min="4" max="4" width="145.25" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,22 +1048,28 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1034,13 +1077,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1048,13 +1094,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1062,19 +1111,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1082,218 +1128,327 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="E36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="E40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>